<commit_message>
review insurance contract section
</commit_message>
<xml_diff>
--- a/Modules/Oje.Section.InsuranceContractBaseData/wwwroot/InsuranceContractBaseDataExcelExample/InsuranceContractUser.xlsx
+++ b/Modules/Oje.Section.InsuranceContractBaseData/wwwroot/InsuranceContractBaseDataExcelExample/InsuranceContractUser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllProje\Fanavaran\Modules\Fanavaran.Section.InsuranceContractBaseData\wwwroot\InsuranceContractBaseDataExcelExample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Oje\Modules\Oje.Section.InsuranceContractBaseData\wwwroot\InsuranceContractBaseDataExcelExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DC5742-8AA4-46B8-8099-7FFA6944E64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B532A78A-6CB8-46C0-ABBD-62EE4B0BAF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>شناسه</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>کد الکترونیکی</t>
   </si>
@@ -42,21 +39,12 @@
     <t>شماره شبا</t>
   </si>
   <si>
-    <t>کد ملی نفر اصلی</t>
-  </si>
-  <si>
-    <t>کد الکترونیکی نفر اصلی</t>
-  </si>
-  <si>
     <t>وضعیت</t>
   </si>
   <si>
     <t>True/False</t>
   </si>
   <si>
-    <t>خالی</t>
-  </si>
-  <si>
     <t>تست</t>
   </si>
   <si>
@@ -69,9 +57,6 @@
     <t>1365/01/01</t>
   </si>
   <si>
-    <t>1 = asli or 2 = hamsar or 3 = farzand pesar or 4 = frarzand dokhtar or 5 = pedar or 6 = madar or 7 = naveh</t>
-  </si>
-  <si>
     <t>شناسه قرارداد*</t>
   </si>
   <si>
@@ -84,13 +69,43 @@
     <t>کد ملی *</t>
   </si>
   <si>
-    <t>نصبت *</t>
-  </si>
-  <si>
-    <t>ایمیل *</t>
-  </si>
-  <si>
     <t>شماره همراه *</t>
+  </si>
+  <si>
+    <t>نام پدر</t>
+  </si>
+  <si>
+    <t>شماره شناسنامه</t>
+  </si>
+  <si>
+    <t>تاریخ استخدام</t>
+  </si>
+  <si>
+    <t>کد جنسیت</t>
+  </si>
+  <si>
+    <t>0 = namoshakhas, 1 = mard, 2 = zan</t>
+  </si>
+  <si>
+    <t>وضعیت تاهل</t>
+  </si>
+  <si>
+    <t>0 = namoshakhas, 1 = mojarad, 2 = motahel, 3 = motalegheh, 4 = moayal</t>
+  </si>
+  <si>
+    <t>شناسه زیرگروه</t>
+  </si>
+  <si>
+    <t>شناسه نوع بیمه</t>
+  </si>
+  <si>
+    <t>شماره دفترچه بیمه پایه</t>
+  </si>
+  <si>
+    <t>کد بانک</t>
+  </si>
+  <si>
+    <t>تلفن ثابت</t>
   </si>
 </sst>
 </file>
@@ -410,103 +425,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="92.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="22" style="1" customWidth="1"/>
+    <col min="16" max="17" width="16.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" t="s">
         <v>5</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
-        <v>123</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix small bugs and missing parts
</commit_message>
<xml_diff>
--- a/Modules/Oje.Section.InsuranceContractBaseData/wwwroot/InsuranceContractBaseDataExcelExample/InsuranceContractUser.xlsx
+++ b/Modules/Oje.Section.InsuranceContractBaseData/wwwroot/InsuranceContractBaseDataExcelExample/InsuranceContractUser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Oje\Modules\Oje.Section.InsuranceContractBaseData\wwwroot\InsuranceContractBaseDataExcelExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B532A78A-6CB8-46C0-ABBD-62EE4B0BAF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BD011F-FFFF-4178-9E92-D9C197829021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>کد الکترونیکی</t>
   </si>
@@ -106,16 +106,33 @@
   </si>
   <si>
     <t>تلفن ثابت</t>
+  </si>
+  <si>
+    <t>کلمه عبور</t>
+  </si>
+  <si>
+    <t>ASE!@#123</t>
+  </si>
+  <si>
+    <t>sh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,15 +155,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,134 +445,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="22" style="1" customWidth="1"/>
-    <col min="16" max="17" width="16.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="22" style="1" customWidth="1"/>
+    <col min="17" max="18" width="16.140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>123</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" t="s">
+      <c r="P2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" t="s">
         <v>5</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" xr:uid="{BDA41420-3285-4D80-A88E-FF10CCA876A0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>